<commit_message>
Klickabfolge an XML angepasst
Codegenerator ignoriert nun fehlerhafte Codes, n2n-Array für längere
Rätsel erweitert, Klickabfolge in XML Szene1 übertragen.
</commit_message>
<xml_diff>
--- a/Klickabfolge Tabelle Szene 1-3.xlsx
+++ b/Klickabfolge Tabelle Szene 1-3.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vendetta1987\Documents\GitHub\MMProject12\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28725" yWindow="-15" windowWidth="19170" windowHeight="12660" activeTab="2"/>
+    <workbookView xWindow="28725" yWindow="-15" windowWidth="19170" windowHeight="12660"/>
   </bookViews>
   <sheets>
     <sheet name="Szene 1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="83">
   <si>
     <t>Interact</t>
   </si>
@@ -81,9 +86,6 @@
     <t>Lautsprecher sound</t>
   </si>
   <si>
-    <t>Schrank</t>
-  </si>
-  <si>
     <t>Mülleimer</t>
   </si>
   <si>
@@ -105,9 +107,6 @@
     <t>"Private"</t>
   </si>
   <si>
-    <t>Dialog on Trigger</t>
-  </si>
-  <si>
     <t>Dialog hat KEIN Trigger</t>
   </si>
   <si>
@@ -232,13 +231,52 @@
   </si>
   <si>
     <t>3.5</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>t|</t>
+  </si>
+  <si>
+    <t>f|</t>
+  </si>
+  <si>
+    <t>raetsel_sichtbar</t>
+  </si>
+  <si>
+    <t>klickbar</t>
+  </si>
+  <si>
+    <t>walkto</t>
+  </si>
+  <si>
+    <t>Dialog on raetsel_ausloeser</t>
+  </si>
+  <si>
+    <t>Dialog hat KEIN raetsel_ausloeser</t>
+  </si>
+  <si>
+    <t>raetsel_ausloeser</t>
+  </si>
+  <si>
+    <t>SZENE 1</t>
+  </si>
+  <si>
+    <t>Schrank zu</t>
+  </si>
+  <si>
+    <t>Schrank offen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,8 +328,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +374,14 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -362,6 +419,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -371,7 +497,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
@@ -384,6 +510,13 @@
     <xf numFmtId="49" fontId="5" fillId="6" borderId="2" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Ausgabe" xfId="5" builtinId="21"/>
@@ -398,6 +531,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -446,7 +582,7 @@
     </a:clrScheme>
     <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -481,7 +617,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -690,25 +826,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA53"/>
+  <dimension ref="A1:AA58"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:N53"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>80</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
@@ -752,25 +931,25 @@
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -789,96 +968,183 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F7" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="G8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -899,103 +1165,179 @@
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="H10" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="H11" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="H12" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="H13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="14" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1017,129 +1359,183 @@
     </row>
     <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F16" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F17" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="J18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="19" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1157,77 +1553,179 @@
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="N20" s="7" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="23" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="24" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1249,103 +1747,183 @@
     </row>
     <row r="25" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N25" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="26" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="27" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="28" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="29" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1363,236 +1941,378 @@
     </row>
     <row r="30" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="K30" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="H31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="32" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="H32" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-    </row>
-    <row r="33" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-    </row>
-    <row r="34" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="K33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="L33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="M33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="N33" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-    </row>
-    <row r="35" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="17"/>
+    </row>
+    <row r="35" spans="1:27" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J35" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="K35" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="M35" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F36" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="37" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F37" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="38" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="K38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="L38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="M38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="N38" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1606,154 +2326,187 @@
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
-      <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-      <c r="Z39" s="4"/>
-      <c r="AA39" s="4"/>
-    </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="N39" s="6"/>
+    </row>
+    <row r="40" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="K40" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
-      <c r="W40" s="2"/>
-      <c r="X40" s="2"/>
-      <c r="Y40" s="2"/>
-      <c r="Z40" s="2"/>
-      <c r="AA40" s="2"/>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="2"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="2"/>
-      <c r="U41" s="2"/>
-      <c r="V41" s="2"/>
-      <c r="W41" s="2"/>
-      <c r="X41" s="2"/>
-      <c r="Y41" s="2"/>
-      <c r="Z41" s="2"/>
-      <c r="AA41" s="2"/>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L41" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M41" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="2"/>
-      <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
-      <c r="W42" s="2"/>
-      <c r="X42" s="2"/>
-      <c r="Y42" s="2"/>
-      <c r="Z42" s="2"/>
-      <c r="AA42" s="2"/>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L42" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M42" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="2"/>
-      <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
-      <c r="W43" s="2"/>
-      <c r="X43" s="2"/>
-      <c r="Y43" s="2"/>
-      <c r="Z43" s="2"/>
-      <c r="AA43" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L43" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M43" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1784,27 +2537,47 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="K45" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="M45" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N45" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
@@ -1821,27 +2594,47 @@
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="K46" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="L46" s="7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="M46" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N46" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
@@ -1858,21 +2651,47 @@
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="N47" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
@@ -1889,23 +2708,47 @@
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="L48" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
@@ -1922,7 +2765,7 @@
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1953,27 +2796,47 @@
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="K50" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="M50" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N50" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
@@ -1990,27 +2853,47 @@
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="K51" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="L51" s="7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="M51" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N51" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
@@ -2027,21 +2910,47 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
@@ -2058,23 +2967,47 @@
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L53" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="M53" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N53" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="N53" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
@@ -2089,9 +3022,268 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
     </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="4"/>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="4"/>
+      <c r="Z54" s="4"/>
+      <c r="AA54" s="4"/>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L55" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="M55" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N55" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+      <c r="V55" s="2"/>
+      <c r="W55" s="2"/>
+      <c r="X55" s="2"/>
+      <c r="Y55" s="2"/>
+      <c r="Z55" s="2"/>
+      <c r="AA55" s="2"/>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L56" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
+      <c r="X56" s="2"/>
+      <c r="Y56" s="2"/>
+      <c r="Z56" s="2"/>
+      <c r="AA56" s="2"/>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M57" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+      <c r="U57" s="2"/>
+      <c r="V57" s="2"/>
+      <c r="W57" s="2"/>
+      <c r="X57" s="2"/>
+      <c r="Y57" s="2"/>
+      <c r="Z57" s="2"/>
+      <c r="AA57" s="2"/>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M58" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
+      <c r="S58" s="2"/>
+      <c r="T58" s="2"/>
+      <c r="U58" s="2"/>
+      <c r="V58" s="2"/>
+      <c r="W58" s="2"/>
+      <c r="X58" s="2"/>
+      <c r="Y58" s="2"/>
+      <c r="Z58" s="2"/>
+      <c r="AA58" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2110,7 +3302,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2128,28 +3320,28 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -2160,10 +3352,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2180,7 +3372,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2201,25 +3393,25 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -2234,7 +3426,7 @@
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -2254,7 +3446,7 @@
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -2273,10 +3465,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -2292,7 +3484,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2313,25 +3505,25 @@
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -2346,10 +3538,10 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2367,13 +3559,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2393,7 +3585,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2408,7 +3600,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -2432,7 +3624,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -2500,7 +3692,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -2525,7 +3717,7 @@
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -2592,7 +3784,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -2616,7 +3808,7 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
@@ -2636,7 +3828,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
@@ -2674,7 +3866,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
@@ -2688,7 +3880,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -2712,7 +3904,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
@@ -2732,7 +3924,7 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -2770,7 +3962,7 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
@@ -2784,7 +3976,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -2809,7 +4001,7 @@
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
@@ -2829,7 +4021,7 @@
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
@@ -2867,7 +4059,7 @@
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
@@ -2880,7 +4072,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -2906,7 +4098,7 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -2972,7 +4164,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -2998,7 +4190,7 @@
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
@@ -3018,7 +4210,7 @@
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
@@ -3056,7 +4248,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
@@ -3068,7 +4260,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -3091,16 +4283,16 @@
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -3166,7 +4358,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -3187,10 +4379,10 @@
         <v>1</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -3347,7 +4539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -3358,7 +4550,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3376,31 +4568,31 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -3410,23 +4602,23 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -3436,7 +4628,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -3457,28 +4649,28 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -3491,7 +4683,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -3511,7 +4703,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -3531,7 +4723,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -3548,7 +4740,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="8"/>
@@ -3570,25 +4762,25 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -3652,7 +4844,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="8"/>
@@ -3674,25 +4866,25 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -3706,7 +4898,7 @@
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -3744,7 +4936,7 @@
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -3760,7 +4952,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="8"/>
@@ -3782,22 +4974,22 @@
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
@@ -3812,7 +5004,7 @@
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -3850,7 +5042,7 @@
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -3866,7 +5058,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -3886,25 +5078,25 @@
       <c r="A25" s="2"/>
       <c r="B25" s="7"/>
       <c r="C25" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -3916,7 +5108,7 @@
       <c r="A26" s="2"/>
       <c r="B26" s="7"/>
       <c r="C26" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -3950,7 +5142,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="7"/>
       <c r="C28" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -3966,7 +5158,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="8"/>
@@ -3988,22 +5180,22 @@
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
@@ -4018,7 +5210,7 @@
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -4056,7 +5248,7 @@
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -4072,7 +5264,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="8"/>
@@ -4100,7 +5292,7 @@
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
@@ -4164,7 +5356,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="8"/>
@@ -4190,10 +5382,10 @@
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
@@ -4258,7 +5450,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="8"/>
@@ -4284,10 +5476,10 @@
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
@@ -4306,7 +5498,7 @@
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
@@ -4344,7 +5536,7 @@
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
@@ -4356,7 +5548,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="8"/>
@@ -4382,10 +5574,10 @@
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I50" s="10"/>
       <c r="J50" s="10"/>
@@ -4405,7 +5597,7 @@
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
       <c r="H51" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="10"/>
@@ -4443,7 +5635,7 @@
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
       <c r="H53" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="10"/>
@@ -4454,7 +5646,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="8"/>
@@ -4473,28 +5665,28 @@
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H55" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>

</xml_diff>